<commit_message>
improve documentation, add benchmark logic
</commit_message>
<xml_diff>
--- a/reports/benchmark.xlsx
+++ b/reports/benchmark.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Philipp\Documents\WU\bachelorarbeit\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0063CDE-7155-48B9-98F5-9F99A1FEDCFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BBBC605-882D-47E6-8067-7297496413C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="50">
   <si>
     <t>ilp</t>
   </si>
@@ -174,6 +174,24 @@
   </si>
   <si>
     <t>% of score hill climbing v1</t>
+  </si>
+  <si>
+    <t>FIXED_TIME_CONSTRAINTS: {
+    7: -100,
+    8: -100, 
+    9: 50,
+    10: 75,
+    11: 75,
+    18: -50,
+    19: -50,
+    20: -75,
+}</t>
+  </si>
+  <si>
+    <t>HOUR_LOAD_CONSTRAINT = (4, 45)</t>
+  </si>
+  <si>
+    <t>COURSE_COUNT_CONSTRAINT = (1, 13)</t>
   </si>
 </sst>
 </file>
@@ -238,17 +256,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -336,7 +355,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-AT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -366,7 +385,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$4:$C$15</c:f>
+              <c:f>Sheet1!$C$8:$C$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -436,7 +455,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$I$4:$I$15</c:f>
+              <c:f>Sheet1!$I$8:$I$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -506,7 +525,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$O$4:$O$15</c:f>
+              <c:f>Sheet1!$O$8:$O$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -827,7 +846,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-AT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -857,7 +876,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$U$4:$U$15</c:f>
+              <c:f>Sheet1!$U$8:$U$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -927,7 +946,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$V$4:$V$15</c:f>
+              <c:f>Sheet1!$V$8:$V$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -1248,7 +1267,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-AT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1278,7 +1297,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$L$4:$L$15</c:f>
+              <c:f>Sheet1!$L$8:$L$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -1348,7 +1367,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$R$4:$R$15</c:f>
+              <c:f>Sheet1!$R$8:$R$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -3273,13 +3292,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3309,13 +3328,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>447675</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3345,13 +3364,13 @@
     <xdr:from>
       <xdr:col>16</xdr:col>
       <xdr:colOff>276225</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
       <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>142876</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3665,913 +3684,928 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V15"/>
+  <dimension ref="A1:V19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
-      <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
+      <c r="A1" s="4" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="U2" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="V2" s="3" t="s">
-        <v>46</v>
+      <c r="A2" t="s">
+        <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>0</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>2050</v>
-      </c>
-      <c r="D4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4">
-        <v>6993170840</v>
-      </c>
-      <c r="G4">
-        <v>161219967.14722711</v>
-      </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-      <c r="I4">
-        <v>2050</v>
-      </c>
-      <c r="J4" t="b">
-        <v>1</v>
-      </c>
-      <c r="K4" t="s">
-        <v>10</v>
-      </c>
-      <c r="L4">
-        <v>11578820</v>
-      </c>
-      <c r="M4">
-        <v>352094.84091647808</v>
-      </c>
-      <c r="N4">
-        <v>1</v>
-      </c>
-      <c r="O4">
-        <v>2050</v>
-      </c>
-      <c r="P4" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>11</v>
-      </c>
-      <c r="R4">
-        <v>13574040</v>
-      </c>
-      <c r="S4">
-        <v>976079.39379950031</v>
-      </c>
-      <c r="U4">
-        <f>I4/C4</f>
-        <v>1</v>
-      </c>
-      <c r="V4">
-        <f>O4/C4</f>
-        <v>1</v>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+      <c r="A5" s="1"/>
+      <c r="B5" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B5">
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C5">
-        <v>4075</v>
-      </c>
-      <c r="D5" t="b">
-        <v>1</v>
-      </c>
-      <c r="E5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5">
-        <v>6067480500</v>
-      </c>
-      <c r="G5">
-        <v>45811293.443429433</v>
-      </c>
-      <c r="H5">
-        <v>2</v>
-      </c>
-      <c r="I5">
-        <v>4075</v>
-      </c>
-      <c r="J5" t="b">
-        <v>1</v>
-      </c>
-      <c r="K5" t="s">
-        <v>13</v>
-      </c>
-      <c r="L5">
-        <v>26824820</v>
-      </c>
-      <c r="M5">
-        <v>2935645.5928807212</v>
-      </c>
-      <c r="N5">
-        <v>2</v>
-      </c>
-      <c r="O5">
-        <v>4075</v>
-      </c>
-      <c r="P5" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>14</v>
-      </c>
-      <c r="R5">
-        <v>32261640</v>
-      </c>
-      <c r="S5">
-        <v>2013683.616658784</v>
-      </c>
-      <c r="U5">
-        <f t="shared" ref="U5:U15" si="0">I5/C5</f>
-        <v>1</v>
-      </c>
-      <c r="V5">
-        <f t="shared" ref="V5:V15" si="1">O5/C5</f>
-        <v>1</v>
-      </c>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="3"/>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>2</v>
-      </c>
-      <c r="B6">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C6">
-        <v>5950</v>
-      </c>
-      <c r="D6" t="b">
-        <v>1</v>
-      </c>
-      <c r="E6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6">
-        <v>6171032400</v>
-      </c>
-      <c r="G6">
-        <v>111165704.5792001</v>
-      </c>
-      <c r="H6">
+      <c r="C6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I6">
-        <v>4825</v>
-      </c>
-      <c r="J6" t="b">
-        <v>1</v>
-      </c>
-      <c r="K6" t="s">
-        <v>16</v>
-      </c>
-      <c r="L6">
-        <v>37763960</v>
-      </c>
-      <c r="M6">
-        <v>2460584.2838643021</v>
-      </c>
-      <c r="N6">
+      <c r="I6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="O6">
-        <v>5575</v>
-      </c>
-      <c r="P6" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>17</v>
-      </c>
-      <c r="R6">
-        <v>56555100</v>
-      </c>
-      <c r="S6">
-        <v>2190849.0066638552</v>
-      </c>
-      <c r="U6">
-        <f t="shared" si="0"/>
-        <v>0.81092436974789917</v>
-      </c>
-      <c r="V6">
-        <f t="shared" si="1"/>
-        <v>0.93697478991596639</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>3</v>
-      </c>
-      <c r="B7">
+      <c r="O6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C7">
-        <v>7450</v>
-      </c>
-      <c r="D7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F7">
-        <v>6253360900</v>
-      </c>
-      <c r="G7">
-        <v>83428330.939825237</v>
-      </c>
-      <c r="H7">
-        <v>4</v>
-      </c>
-      <c r="I7">
-        <v>6225</v>
-      </c>
-      <c r="J7" t="b">
-        <v>1</v>
-      </c>
-      <c r="K7" t="s">
-        <v>19</v>
-      </c>
-      <c r="L7">
-        <v>49514320</v>
-      </c>
-      <c r="M7">
-        <v>6704127.3352316329</v>
-      </c>
-      <c r="N7">
-        <v>4</v>
-      </c>
-      <c r="O7">
-        <v>6725</v>
-      </c>
-      <c r="P7" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>20</v>
-      </c>
-      <c r="R7">
-        <v>81531540</v>
-      </c>
-      <c r="S7">
-        <v>1548801.5440978869</v>
-      </c>
-      <c r="U7">
-        <f t="shared" si="0"/>
-        <v>0.83557046979865768</v>
-      </c>
-      <c r="V7">
-        <f t="shared" si="1"/>
-        <v>0.90268456375838924</v>
+      <c r="P6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="U6" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="V6" s="2" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B8">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C8">
-        <v>8950</v>
+        <v>2050</v>
       </c>
       <c r="D8" t="b">
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="F8">
-        <v>6286068380</v>
+        <v>6993170840</v>
       </c>
       <c r="G8">
-        <v>68822965.859529763</v>
+        <v>161219967.14722711</v>
       </c>
       <c r="H8">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I8">
-        <v>6225</v>
+        <v>2050</v>
       </c>
       <c r="J8" t="b">
         <v>1</v>
       </c>
       <c r="K8" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="L8">
-        <v>53398900</v>
+        <v>11578820</v>
       </c>
       <c r="M8">
-        <v>2307610.4404773349</v>
+        <v>352094.84091647808</v>
       </c>
       <c r="N8">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="O8">
-        <v>7725</v>
+        <v>2050</v>
       </c>
       <c r="P8" t="b">
         <v>1</v>
       </c>
       <c r="Q8" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="R8">
-        <v>111265700</v>
+        <v>13574040</v>
       </c>
       <c r="S8">
-        <v>2198831.0178365228</v>
+        <v>976079.39379950031</v>
       </c>
       <c r="U8">
-        <f t="shared" si="0"/>
-        <v>0.6955307262569832</v>
+        <f>I8/C8</f>
+        <v>1</v>
       </c>
       <c r="V8">
-        <f t="shared" si="1"/>
-        <v>0.86312849162011174</v>
+        <f>O8/C8</f>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B9">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C9">
-        <v>9950</v>
+        <v>4075</v>
       </c>
       <c r="D9" t="b">
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F9">
-        <v>6289775740</v>
+        <v>6067480500</v>
       </c>
       <c r="G9">
-        <v>139481002.73911139</v>
+        <v>45811293.443429433</v>
       </c>
       <c r="H9">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="I9">
-        <v>6675</v>
+        <v>4075</v>
       </c>
       <c r="J9" t="b">
         <v>1</v>
       </c>
       <c r="K9" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="L9">
-        <v>55100760</v>
+        <v>26824820</v>
       </c>
       <c r="M9">
-        <v>2384431.643599791</v>
+        <v>2935645.5928807212</v>
       </c>
       <c r="N9">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="O9">
-        <v>8475</v>
+        <v>4075</v>
       </c>
       <c r="P9" t="b">
         <v>1</v>
       </c>
       <c r="Q9" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="R9">
-        <v>153826380</v>
+        <v>32261640</v>
       </c>
       <c r="S9">
-        <v>8168981.6242295466</v>
+        <v>2013683.616658784</v>
       </c>
       <c r="U9">
-        <f t="shared" si="0"/>
-        <v>0.67085427135678388</v>
+        <f t="shared" ref="U9:U19" si="0">I9/C9</f>
+        <v>1</v>
       </c>
       <c r="V9">
-        <f t="shared" si="1"/>
-        <v>0.85175879396984921</v>
+        <f t="shared" ref="V9:V19" si="1">O9/C9</f>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B10">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C10">
-        <v>10950</v>
+        <v>5950</v>
       </c>
       <c r="D10" t="b">
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="F10">
-        <v>6373218060</v>
+        <v>6171032400</v>
       </c>
       <c r="G10">
-        <v>173448631.53747571</v>
+        <v>111165704.5792001</v>
       </c>
       <c r="H10">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="I10">
-        <v>7825</v>
+        <v>4825</v>
       </c>
       <c r="J10" t="b">
         <v>1</v>
       </c>
       <c r="K10" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="L10">
-        <v>43976440</v>
+        <v>37763960</v>
       </c>
       <c r="M10">
-        <v>2727571.1334445518</v>
+        <v>2460584.2838643021</v>
       </c>
       <c r="N10">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="O10">
-        <v>8875</v>
+        <v>5575</v>
       </c>
       <c r="P10" t="b">
         <v>1</v>
       </c>
       <c r="Q10" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="R10">
-        <v>173297460</v>
+        <v>56555100</v>
       </c>
       <c r="S10">
-        <v>5013891.5677345879</v>
+        <v>2190849.0066638552</v>
       </c>
       <c r="U10">
         <f t="shared" si="0"/>
-        <v>0.71461187214611877</v>
+        <v>0.81092436974789917</v>
       </c>
       <c r="V10">
         <f t="shared" si="1"/>
-        <v>0.81050228310502281</v>
+        <v>0.93697478991596639</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B11">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C11">
-        <v>11350</v>
+        <v>7450</v>
       </c>
       <c r="D11" t="b">
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="F11">
-        <v>6581105660</v>
+        <v>6253360900</v>
       </c>
       <c r="G11">
-        <v>188407433.07663849</v>
+        <v>83428330.939825237</v>
       </c>
       <c r="H11">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="I11">
-        <v>7950</v>
+        <v>6225</v>
       </c>
       <c r="J11" t="b">
         <v>1</v>
       </c>
       <c r="K11" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="L11">
-        <v>43582360</v>
+        <v>49514320</v>
       </c>
       <c r="M11">
-        <v>3687549.0855038119</v>
+        <v>6704127.3352316329</v>
       </c>
       <c r="N11">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="O11">
-        <v>9025</v>
+        <v>6725</v>
       </c>
       <c r="P11" t="b">
         <v>1</v>
       </c>
       <c r="Q11" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="R11">
-        <v>190258660</v>
+        <v>81531540</v>
       </c>
       <c r="S11">
-        <v>4442726.4335090453</v>
+        <v>1548801.5440978869</v>
       </c>
       <c r="U11">
         <f t="shared" si="0"/>
-        <v>0.70044052863436124</v>
+        <v>0.83557046979865768</v>
       </c>
       <c r="V11">
         <f t="shared" si="1"/>
-        <v>0.79515418502202639</v>
+        <v>0.90268456375838924</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B12">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C12">
-        <v>11475</v>
+        <v>8950</v>
       </c>
       <c r="D12" t="b">
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="F12">
-        <v>6631693500</v>
+        <v>6286068380</v>
       </c>
       <c r="G12">
-        <v>155159686.43238169</v>
+        <v>68822965.859529763</v>
       </c>
       <c r="H12">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="I12">
-        <v>8075</v>
+        <v>6225</v>
       </c>
       <c r="J12" t="b">
         <v>1</v>
       </c>
       <c r="K12" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="L12">
-        <v>45893360</v>
+        <v>53398900</v>
       </c>
       <c r="M12">
-        <v>5517285.5801562415</v>
+        <v>2307610.4404773349</v>
       </c>
       <c r="N12">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="O12">
-        <v>9025</v>
+        <v>7725</v>
       </c>
       <c r="P12" t="b">
         <v>1</v>
       </c>
       <c r="Q12" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="R12">
-        <v>206657280</v>
+        <v>111265700</v>
       </c>
       <c r="S12">
-        <v>2685045.119173978</v>
+        <v>2198831.0178365228</v>
       </c>
       <c r="U12">
         <f t="shared" si="0"/>
-        <v>0.70370370370370372</v>
+        <v>0.6955307262569832</v>
       </c>
       <c r="V12">
         <f t="shared" si="1"/>
-        <v>0.78649237472766886</v>
+        <v>0.86312849162011174</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B13">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C13">
-        <v>11600</v>
+        <v>9950</v>
       </c>
       <c r="D13" t="b">
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="F13">
-        <v>6657019420</v>
+        <v>6289775740</v>
       </c>
       <c r="G13">
-        <v>173239407.04079711</v>
+        <v>139481002.73911139</v>
       </c>
       <c r="H13">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="I13">
-        <v>8475</v>
+        <v>6675</v>
       </c>
       <c r="J13" t="b">
         <v>1</v>
       </c>
       <c r="K13" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="L13">
-        <v>28554100</v>
+        <v>55100760</v>
       </c>
       <c r="M13">
-        <v>1374291.004481948</v>
+        <v>2384431.643599791</v>
       </c>
       <c r="N13">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="O13">
-        <v>9025</v>
+        <v>8475</v>
       </c>
       <c r="P13" t="b">
         <v>1</v>
       </c>
       <c r="Q13" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="R13">
-        <v>218618860</v>
+        <v>153826380</v>
       </c>
       <c r="S13">
-        <v>9207895.62022724</v>
+        <v>8168981.6242295466</v>
       </c>
       <c r="U13">
         <f t="shared" si="0"/>
-        <v>0.7306034482758621</v>
+        <v>0.67085427135678388</v>
       </c>
       <c r="V13">
         <f t="shared" si="1"/>
-        <v>0.77801724137931039</v>
+        <v>0.85175879396984921</v>
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B14">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C14">
-        <v>11600</v>
+        <v>10950</v>
       </c>
       <c r="D14" t="b">
         <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="F14">
-        <v>9702281300</v>
+        <v>6373218060</v>
       </c>
       <c r="G14">
-        <v>316659027.06926727</v>
+        <v>173448631.53747571</v>
       </c>
       <c r="H14">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="I14">
-        <v>7925</v>
+        <v>7825</v>
       </c>
       <c r="J14" t="b">
         <v>1</v>
       </c>
       <c r="K14" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="L14">
-        <v>29544700</v>
+        <v>43976440</v>
       </c>
       <c r="M14">
-        <v>2511521.0381360529</v>
+        <v>2727571.1334445518</v>
       </c>
       <c r="N14">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="O14">
-        <v>8975</v>
+        <v>8875</v>
       </c>
       <c r="P14" t="b">
         <v>1</v>
       </c>
       <c r="Q14" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="R14">
-        <v>220807920</v>
+        <v>173297460</v>
       </c>
       <c r="S14">
-        <v>6106007.3765104478</v>
+        <v>5013891.5677345879</v>
       </c>
       <c r="U14">
         <f t="shared" si="0"/>
-        <v>0.68318965517241381</v>
+        <v>0.71461187214611877</v>
       </c>
       <c r="V14">
         <f t="shared" si="1"/>
-        <v>0.77370689655172409</v>
+        <v>0.81050228310502281</v>
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B15">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C15">
-        <v>11600</v>
+        <v>11350</v>
       </c>
       <c r="D15" t="b">
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="F15">
-        <v>9517605000</v>
+        <v>6581105660</v>
       </c>
       <c r="G15">
-        <v>71575243.936887845</v>
+        <v>188407433.07663849</v>
       </c>
       <c r="H15">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="I15">
-        <v>7425</v>
+        <v>7950</v>
       </c>
       <c r="J15" t="b">
         <v>1</v>
       </c>
       <c r="K15" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="L15">
-        <v>141190560</v>
+        <v>43582360</v>
       </c>
       <c r="M15">
-        <v>4807991.0865142001</v>
+        <v>3687549.0855038119</v>
       </c>
       <c r="N15">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="O15">
-        <v>8400</v>
+        <v>9025</v>
       </c>
       <c r="P15" t="b">
         <v>1</v>
       </c>
       <c r="Q15" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="R15">
-        <v>225462480</v>
+        <v>190258660</v>
       </c>
       <c r="S15">
-        <v>5057501.4772118451</v>
+        <v>4442726.4335090453</v>
       </c>
       <c r="U15">
         <f t="shared" si="0"/>
+        <v>0.70044052863436124</v>
+      </c>
+      <c r="V15">
+        <f t="shared" si="1"/>
+        <v>0.79515418502202639</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>8</v>
+      </c>
+      <c r="B16">
+        <v>9</v>
+      </c>
+      <c r="C16">
+        <v>11475</v>
+      </c>
+      <c r="D16" t="b">
+        <v>1</v>
+      </c>
+      <c r="E16" t="s">
+        <v>33</v>
+      </c>
+      <c r="F16">
+        <v>6631693500</v>
+      </c>
+      <c r="G16">
+        <v>155159686.43238169</v>
+      </c>
+      <c r="H16">
+        <v>9</v>
+      </c>
+      <c r="I16">
+        <v>8075</v>
+      </c>
+      <c r="J16" t="b">
+        <v>1</v>
+      </c>
+      <c r="K16" t="s">
+        <v>34</v>
+      </c>
+      <c r="L16">
+        <v>45893360</v>
+      </c>
+      <c r="M16">
+        <v>5517285.5801562415</v>
+      </c>
+      <c r="N16">
+        <v>9</v>
+      </c>
+      <c r="O16">
+        <v>9025</v>
+      </c>
+      <c r="P16" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>35</v>
+      </c>
+      <c r="R16">
+        <v>206657280</v>
+      </c>
+      <c r="S16">
+        <v>2685045.119173978</v>
+      </c>
+      <c r="U16">
+        <f t="shared" si="0"/>
+        <v>0.70370370370370372</v>
+      </c>
+      <c r="V16">
+        <f t="shared" si="1"/>
+        <v>0.78649237472766886</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>9</v>
+      </c>
+      <c r="B17">
+        <v>10</v>
+      </c>
+      <c r="C17">
+        <v>11600</v>
+      </c>
+      <c r="D17" t="b">
+        <v>1</v>
+      </c>
+      <c r="E17" t="s">
+        <v>36</v>
+      </c>
+      <c r="F17">
+        <v>6657019420</v>
+      </c>
+      <c r="G17">
+        <v>173239407.04079711</v>
+      </c>
+      <c r="H17">
+        <v>10</v>
+      </c>
+      <c r="I17">
+        <v>8475</v>
+      </c>
+      <c r="J17" t="b">
+        <v>1</v>
+      </c>
+      <c r="K17" t="s">
+        <v>37</v>
+      </c>
+      <c r="L17">
+        <v>28554100</v>
+      </c>
+      <c r="M17">
+        <v>1374291.004481948</v>
+      </c>
+      <c r="N17">
+        <v>10</v>
+      </c>
+      <c r="O17">
+        <v>9025</v>
+      </c>
+      <c r="P17" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>38</v>
+      </c>
+      <c r="R17">
+        <v>218618860</v>
+      </c>
+      <c r="S17">
+        <v>9207895.62022724</v>
+      </c>
+      <c r="U17">
+        <f t="shared" si="0"/>
+        <v>0.7306034482758621</v>
+      </c>
+      <c r="V17">
+        <f t="shared" si="1"/>
+        <v>0.77801724137931039</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>10</v>
+      </c>
+      <c r="B18">
+        <v>11</v>
+      </c>
+      <c r="C18">
+        <v>11600</v>
+      </c>
+      <c r="D18" t="b">
+        <v>1</v>
+      </c>
+      <c r="E18" t="s">
+        <v>39</v>
+      </c>
+      <c r="F18">
+        <v>9702281300</v>
+      </c>
+      <c r="G18">
+        <v>316659027.06926727</v>
+      </c>
+      <c r="H18">
+        <v>11</v>
+      </c>
+      <c r="I18">
+        <v>7925</v>
+      </c>
+      <c r="J18" t="b">
+        <v>1</v>
+      </c>
+      <c r="K18" t="s">
+        <v>40</v>
+      </c>
+      <c r="L18">
+        <v>29544700</v>
+      </c>
+      <c r="M18">
+        <v>2511521.0381360529</v>
+      </c>
+      <c r="N18">
+        <v>11</v>
+      </c>
+      <c r="O18">
+        <v>8975</v>
+      </c>
+      <c r="P18" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>41</v>
+      </c>
+      <c r="R18">
+        <v>220807920</v>
+      </c>
+      <c r="S18">
+        <v>6106007.3765104478</v>
+      </c>
+      <c r="U18">
+        <f t="shared" si="0"/>
+        <v>0.68318965517241381</v>
+      </c>
+      <c r="V18">
+        <f t="shared" si="1"/>
+        <v>0.77370689655172409</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>11</v>
+      </c>
+      <c r="B19">
+        <v>12</v>
+      </c>
+      <c r="C19">
+        <v>11600</v>
+      </c>
+      <c r="D19" t="b">
+        <v>1</v>
+      </c>
+      <c r="E19" t="s">
+        <v>42</v>
+      </c>
+      <c r="F19">
+        <v>9517605000</v>
+      </c>
+      <c r="G19">
+        <v>71575243.936887845</v>
+      </c>
+      <c r="H19">
+        <v>12</v>
+      </c>
+      <c r="I19">
+        <v>7425</v>
+      </c>
+      <c r="J19" t="b">
+        <v>1</v>
+      </c>
+      <c r="K19" t="s">
+        <v>43</v>
+      </c>
+      <c r="L19">
+        <v>141190560</v>
+      </c>
+      <c r="M19">
+        <v>4807991.0865142001</v>
+      </c>
+      <c r="N19">
+        <v>12</v>
+      </c>
+      <c r="O19">
+        <v>8400</v>
+      </c>
+      <c r="P19" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>44</v>
+      </c>
+      <c r="R19">
+        <v>225462480</v>
+      </c>
+      <c r="S19">
+        <v>5057501.4772118451</v>
+      </c>
+      <c r="U19">
+        <f t="shared" si="0"/>
         <v>0.64008620689655171</v>
       </c>
-      <c r="V15">
+      <c r="V19">
         <f t="shared" si="1"/>
         <v>0.72413793103448276</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="N1:S1"/>
-    <mergeCell ref="H1:M1"/>
-    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="N5:S5"/>
+    <mergeCell ref="H5:M5"/>
+    <mergeCell ref="B5:G5"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
improve testing framework, create first real test benchmark with latex compatible output
</commit_message>
<xml_diff>
--- a/reports/benchmark.xlsx
+++ b/reports/benchmark.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Philipp\Documents\WU\bachelorarbeit\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BBBC605-882D-47E6-8067-7297496413C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E71A573B-A80C-4A40-AA42-A12C593E6753}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="53">
   <si>
     <t>ilp</t>
   </si>
@@ -193,11 +193,24 @@
   <si>
     <t>COURSE_COUNT_CONSTRAINT = (1, 13)</t>
   </si>
+  <si>
+    <t>Notiz: In Paper ist offering order besser als hill climbing, bei mir konstant umgekehrt</t>
+  </si>
+  <si>
+    <t>Notiz: Ähnliches Bild wie im paper, hill climbing benötigt mehr Zeit</t>
+  </si>
+  <si>
+    <t>mean (s)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="168" formatCode="0.000"/>
+    <numFmt numFmtId="169" formatCode="0.0"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -256,7 +269,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -267,7 +280,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -455,7 +469,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$I$8:$I$19</c:f>
+              <c:f>Sheet1!$J$8:$J$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -525,7 +539,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$O$8:$O$19</c:f>
+              <c:f>Sheet1!$Q$8:$Q$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -876,7 +890,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$U$8:$U$19</c:f>
+              <c:f>Sheet1!$X$8:$X$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -946,7 +960,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$V$8:$V$19</c:f>
+              <c:f>Sheet1!$Y$8:$Y$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -1297,7 +1311,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$L$8:$L$19</c:f>
+              <c:f>Sheet1!$M$8:$M$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -1367,7 +1381,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$R$8:$R$19</c:f>
+              <c:f>Sheet1!$T$8:$T$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -3296,7 +3310,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>34</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
@@ -3326,13 +3340,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>447675</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>142875</xdr:colOff>
       <xdr:row>34</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
@@ -3362,13 +3376,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>276225</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
+      <xdr:col>28</xdr:col>
       <xdr:colOff>114300</xdr:colOff>
       <xdr:row>34</xdr:row>
       <xdr:rowOff>142876</xdr:rowOff>
@@ -3394,6 +3408,99 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>345681</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>14873</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7D058D06-B46A-AB5A-949D-9E77C5F0D67D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5222481" y="6772275"/>
+          <a:ext cx="4416819" cy="3529598"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>572097</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>29042</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C0AD578B-0695-A9D0-9E7E-1E0158FC8FAC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10315575" y="6781800"/>
+          <a:ext cx="4277322" cy="3343742"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -3684,30 +3791,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V19"/>
+  <dimension ref="A1:Y56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="3" t="s">
         <v>0</v>
@@ -3717,24 +3827,27 @@
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="3"/>
+      <c r="I5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="I5" s="3"/>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
       <c r="M5" s="3"/>
-      <c r="N5" s="3" t="s">
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="O5" s="3"/>
-      <c r="P5" s="3"/>
       <c r="Q5" s="3"/>
       <c r="R5" s="3"/>
       <c r="S5" s="3"/>
+      <c r="T5" s="3"/>
+      <c r="U5" s="3"/>
+      <c r="V5" s="3"/>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
         <v>3</v>
@@ -3752,52 +3865,61 @@
         <v>7</v>
       </c>
       <c r="G6" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="I6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="J6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="K6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="L6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="L6" s="1" t="s">
+      <c r="M6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="M6" s="1" t="s">
+      <c r="N6" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="O6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="N6" s="1" t="s">
+      <c r="P6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="O6" s="1" t="s">
+      <c r="Q6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="P6" s="1" t="s">
+      <c r="R6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="Q6" s="1" t="s">
+      <c r="S6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="R6" s="1" t="s">
+      <c r="T6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="S6" s="1" t="s">
+      <c r="U6" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="V6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="U6" s="2" t="s">
+      <c r="X6" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="V6" s="2" t="s">
+      <c r="Y6" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>0</v>
       </c>
@@ -3816,55 +3938,67 @@
       <c r="F8">
         <v>6993170840</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="5">
+        <f>F8/1000000000</f>
+        <v>6.9931708400000003</v>
+      </c>
+      <c r="H8">
         <v>161219967.14722711</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>1</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>2050</v>
       </c>
-      <c r="J8" t="b">
+      <c r="K8" t="b">
         <v>1</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
         <v>10</v>
       </c>
-      <c r="L8">
+      <c r="M8">
         <v>11578820</v>
       </c>
-      <c r="M8">
+      <c r="N8" s="4">
+        <f>M8/1000000000</f>
+        <v>1.157882E-2</v>
+      </c>
+      <c r="O8">
         <v>352094.84091647808</v>
       </c>
-      <c r="N8">
+      <c r="P8">
         <v>1</v>
       </c>
-      <c r="O8">
+      <c r="Q8">
         <v>2050</v>
       </c>
-      <c r="P8" t="b">
+      <c r="R8" t="b">
         <v>1</v>
       </c>
-      <c r="Q8" t="s">
+      <c r="S8" t="s">
         <v>11</v>
       </c>
-      <c r="R8">
+      <c r="T8">
         <v>13574040</v>
       </c>
-      <c r="S8">
+      <c r="U8" s="4">
+        <f>T8/1000000000</f>
+        <v>1.3574040000000001E-2</v>
+      </c>
+      <c r="V8">
         <v>976079.39379950031</v>
       </c>
-      <c r="U8">
-        <f>I8/C8</f>
+      <c r="X8">
+        <f>J8/C8</f>
         <v>1</v>
       </c>
-      <c r="V8">
-        <f>O8/C8</f>
+      <c r="Y8">
+        <f>Q8/C8</f>
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>1</v>
       </c>
@@ -3883,55 +4017,67 @@
       <c r="F9">
         <v>6067480500</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="5">
+        <f t="shared" ref="G9:G19" si="0">F9/1000000000</f>
+        <v>6.0674805000000003</v>
+      </c>
+      <c r="H9">
         <v>45811293.443429433</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>2</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>4075</v>
       </c>
-      <c r="J9" t="b">
+      <c r="K9" t="b">
         <v>1</v>
       </c>
-      <c r="K9" t="s">
+      <c r="L9" t="s">
         <v>13</v>
       </c>
-      <c r="L9">
+      <c r="M9">
         <v>26824820</v>
       </c>
-      <c r="M9">
+      <c r="N9" s="4">
+        <f t="shared" ref="N9:N19" si="1">M9/1000000000</f>
+        <v>2.6824819999999999E-2</v>
+      </c>
+      <c r="O9">
         <v>2935645.5928807212</v>
       </c>
-      <c r="N9">
+      <c r="P9">
         <v>2</v>
       </c>
-      <c r="O9">
+      <c r="Q9">
         <v>4075</v>
       </c>
-      <c r="P9" t="b">
+      <c r="R9" t="b">
         <v>1</v>
       </c>
-      <c r="Q9" t="s">
+      <c r="S9" t="s">
         <v>14</v>
       </c>
-      <c r="R9">
+      <c r="T9">
         <v>32261640</v>
       </c>
-      <c r="S9">
+      <c r="U9" s="4">
+        <f t="shared" ref="U9:U19" si="2">T9/1000000000</f>
+        <v>3.2261640000000001E-2</v>
+      </c>
+      <c r="V9">
         <v>2013683.616658784</v>
       </c>
-      <c r="U9">
-        <f t="shared" ref="U9:U19" si="0">I9/C9</f>
+      <c r="X9">
+        <f t="shared" ref="X9:X19" si="3">J9/C9</f>
         <v>1</v>
       </c>
-      <c r="V9">
-        <f t="shared" ref="V9:V19" si="1">O9/C9</f>
+      <c r="Y9">
+        <f t="shared" ref="Y9:Y19" si="4">Q9/C9</f>
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>2</v>
       </c>
@@ -3950,55 +4096,67 @@
       <c r="F10">
         <v>6171032400</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="5">
+        <f t="shared" si="0"/>
+        <v>6.1710323999999996</v>
+      </c>
+      <c r="H10">
         <v>111165704.5792001</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>3</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>4825</v>
       </c>
-      <c r="J10" t="b">
+      <c r="K10" t="b">
         <v>1</v>
       </c>
-      <c r="K10" t="s">
+      <c r="L10" t="s">
         <v>16</v>
       </c>
-      <c r="L10">
+      <c r="M10">
         <v>37763960</v>
       </c>
-      <c r="M10">
+      <c r="N10" s="4">
+        <f t="shared" si="1"/>
+        <v>3.7763959999999999E-2</v>
+      </c>
+      <c r="O10">
         <v>2460584.2838643021</v>
       </c>
-      <c r="N10">
+      <c r="P10">
         <v>3</v>
       </c>
-      <c r="O10">
+      <c r="Q10">
         <v>5575</v>
       </c>
-      <c r="P10" t="b">
+      <c r="R10" t="b">
         <v>1</v>
       </c>
-      <c r="Q10" t="s">
+      <c r="S10" t="s">
         <v>17</v>
       </c>
-      <c r="R10">
+      <c r="T10">
         <v>56555100</v>
       </c>
-      <c r="S10">
+      <c r="U10" s="4">
+        <f t="shared" si="2"/>
+        <v>5.6555099999999997E-2</v>
+      </c>
+      <c r="V10">
         <v>2190849.0066638552</v>
       </c>
-      <c r="U10">
-        <f t="shared" si="0"/>
+      <c r="X10">
+        <f t="shared" si="3"/>
         <v>0.81092436974789917</v>
       </c>
-      <c r="V10">
-        <f t="shared" si="1"/>
+      <c r="Y10">
+        <f t="shared" si="4"/>
         <v>0.93697478991596639</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>3</v>
       </c>
@@ -4017,55 +4175,67 @@
       <c r="F11">
         <v>6253360900</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="5">
+        <f t="shared" si="0"/>
+        <v>6.2533608999999997</v>
+      </c>
+      <c r="H11">
         <v>83428330.939825237</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <v>4</v>
       </c>
-      <c r="I11">
+      <c r="J11">
         <v>6225</v>
       </c>
-      <c r="J11" t="b">
+      <c r="K11" t="b">
         <v>1</v>
       </c>
-      <c r="K11" t="s">
+      <c r="L11" t="s">
         <v>19</v>
       </c>
-      <c r="L11">
+      <c r="M11">
         <v>49514320</v>
       </c>
-      <c r="M11">
+      <c r="N11" s="4">
+        <f t="shared" si="1"/>
+        <v>4.9514320000000001E-2</v>
+      </c>
+      <c r="O11">
         <v>6704127.3352316329</v>
       </c>
-      <c r="N11">
+      <c r="P11">
         <v>4</v>
       </c>
-      <c r="O11">
+      <c r="Q11">
         <v>6725</v>
       </c>
-      <c r="P11" t="b">
+      <c r="R11" t="b">
         <v>1</v>
       </c>
-      <c r="Q11" t="s">
+      <c r="S11" t="s">
         <v>20</v>
       </c>
-      <c r="R11">
+      <c r="T11">
         <v>81531540</v>
       </c>
-      <c r="S11">
+      <c r="U11" s="4">
+        <f t="shared" si="2"/>
+        <v>8.153154E-2</v>
+      </c>
+      <c r="V11">
         <v>1548801.5440978869</v>
       </c>
-      <c r="U11">
-        <f t="shared" si="0"/>
+      <c r="X11">
+        <f t="shared" si="3"/>
         <v>0.83557046979865768</v>
       </c>
-      <c r="V11">
-        <f t="shared" si="1"/>
+      <c r="Y11">
+        <f t="shared" si="4"/>
         <v>0.90268456375838924</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>4</v>
       </c>
@@ -4084,55 +4254,67 @@
       <c r="F12">
         <v>6286068380</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="5">
+        <f t="shared" si="0"/>
+        <v>6.2860683799999997</v>
+      </c>
+      <c r="H12">
         <v>68822965.859529763</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <v>5</v>
       </c>
-      <c r="I12">
+      <c r="J12">
         <v>6225</v>
       </c>
-      <c r="J12" t="b">
+      <c r="K12" t="b">
         <v>1</v>
       </c>
-      <c r="K12" t="s">
+      <c r="L12" t="s">
         <v>22</v>
       </c>
-      <c r="L12">
+      <c r="M12">
         <v>53398900</v>
       </c>
-      <c r="M12">
+      <c r="N12" s="4">
+        <f t="shared" si="1"/>
+        <v>5.3398899999999999E-2</v>
+      </c>
+      <c r="O12">
         <v>2307610.4404773349</v>
       </c>
-      <c r="N12">
+      <c r="P12">
         <v>5</v>
       </c>
-      <c r="O12">
+      <c r="Q12">
         <v>7725</v>
       </c>
-      <c r="P12" t="b">
+      <c r="R12" t="b">
         <v>1</v>
       </c>
-      <c r="Q12" t="s">
+      <c r="S12" t="s">
         <v>23</v>
       </c>
-      <c r="R12">
+      <c r="T12">
         <v>111265700</v>
       </c>
-      <c r="S12">
+      <c r="U12" s="4">
+        <f t="shared" si="2"/>
+        <v>0.1112657</v>
+      </c>
+      <c r="V12">
         <v>2198831.0178365228</v>
       </c>
-      <c r="U12">
-        <f t="shared" si="0"/>
+      <c r="X12">
+        <f t="shared" si="3"/>
         <v>0.6955307262569832</v>
       </c>
-      <c r="V12">
-        <f t="shared" si="1"/>
+      <c r="Y12">
+        <f t="shared" si="4"/>
         <v>0.86312849162011174</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>5</v>
       </c>
@@ -4151,55 +4333,67 @@
       <c r="F13">
         <v>6289775740</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="5">
+        <f t="shared" si="0"/>
+        <v>6.2897757399999996</v>
+      </c>
+      <c r="H13">
         <v>139481002.73911139</v>
       </c>
-      <c r="H13">
+      <c r="I13">
         <v>6</v>
       </c>
-      <c r="I13">
+      <c r="J13">
         <v>6675</v>
       </c>
-      <c r="J13" t="b">
+      <c r="K13" t="b">
         <v>1</v>
       </c>
-      <c r="K13" t="s">
+      <c r="L13" t="s">
         <v>25</v>
       </c>
-      <c r="L13">
+      <c r="M13">
         <v>55100760</v>
       </c>
-      <c r="M13">
+      <c r="N13" s="4">
+        <f t="shared" si="1"/>
+        <v>5.5100759999999999E-2</v>
+      </c>
+      <c r="O13">
         <v>2384431.643599791</v>
       </c>
-      <c r="N13">
+      <c r="P13">
         <v>6</v>
       </c>
-      <c r="O13">
+      <c r="Q13">
         <v>8475</v>
       </c>
-      <c r="P13" t="b">
+      <c r="R13" t="b">
         <v>1</v>
       </c>
-      <c r="Q13" t="s">
+      <c r="S13" t="s">
         <v>26</v>
       </c>
-      <c r="R13">
+      <c r="T13">
         <v>153826380</v>
       </c>
-      <c r="S13">
+      <c r="U13" s="4">
+        <f t="shared" si="2"/>
+        <v>0.15382638000000001</v>
+      </c>
+      <c r="V13">
         <v>8168981.6242295466</v>
       </c>
-      <c r="U13">
-        <f t="shared" si="0"/>
+      <c r="X13">
+        <f t="shared" si="3"/>
         <v>0.67085427135678388</v>
       </c>
-      <c r="V13">
-        <f t="shared" si="1"/>
+      <c r="Y13">
+        <f t="shared" si="4"/>
         <v>0.85175879396984921</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>6</v>
       </c>
@@ -4218,55 +4412,67 @@
       <c r="F14">
         <v>6373218060</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="5">
+        <f t="shared" si="0"/>
+        <v>6.3732180600000001</v>
+      </c>
+      <c r="H14">
         <v>173448631.53747571</v>
       </c>
-      <c r="H14">
+      <c r="I14">
         <v>7</v>
       </c>
-      <c r="I14">
+      <c r="J14">
         <v>7825</v>
       </c>
-      <c r="J14" t="b">
+      <c r="K14" t="b">
         <v>1</v>
       </c>
-      <c r="K14" t="s">
+      <c r="L14" t="s">
         <v>28</v>
       </c>
-      <c r="L14">
+      <c r="M14">
         <v>43976440</v>
       </c>
-      <c r="M14">
+      <c r="N14" s="4">
+        <f t="shared" si="1"/>
+        <v>4.3976439999999999E-2</v>
+      </c>
+      <c r="O14">
         <v>2727571.1334445518</v>
       </c>
-      <c r="N14">
+      <c r="P14">
         <v>7</v>
       </c>
-      <c r="O14">
+      <c r="Q14">
         <v>8875</v>
       </c>
-      <c r="P14" t="b">
+      <c r="R14" t="b">
         <v>1</v>
       </c>
-      <c r="Q14" t="s">
+      <c r="S14" t="s">
         <v>29</v>
       </c>
-      <c r="R14">
+      <c r="T14">
         <v>173297460</v>
       </c>
-      <c r="S14">
+      <c r="U14" s="4">
+        <f t="shared" si="2"/>
+        <v>0.17329745999999999</v>
+      </c>
+      <c r="V14">
         <v>5013891.5677345879</v>
       </c>
-      <c r="U14">
-        <f t="shared" si="0"/>
+      <c r="X14">
+        <f t="shared" si="3"/>
         <v>0.71461187214611877</v>
       </c>
-      <c r="V14">
-        <f t="shared" si="1"/>
+      <c r="Y14">
+        <f t="shared" si="4"/>
         <v>0.81050228310502281</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>7</v>
       </c>
@@ -4285,55 +4491,67 @@
       <c r="F15">
         <v>6581105660</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="5">
+        <f t="shared" si="0"/>
+        <v>6.5811056600000004</v>
+      </c>
+      <c r="H15">
         <v>188407433.07663849</v>
       </c>
-      <c r="H15">
+      <c r="I15">
         <v>8</v>
       </c>
-      <c r="I15">
+      <c r="J15">
         <v>7950</v>
       </c>
-      <c r="J15" t="b">
+      <c r="K15" t="b">
         <v>1</v>
       </c>
-      <c r="K15" t="s">
+      <c r="L15" t="s">
         <v>31</v>
       </c>
-      <c r="L15">
+      <c r="M15">
         <v>43582360</v>
       </c>
-      <c r="M15">
+      <c r="N15" s="4">
+        <f t="shared" si="1"/>
+        <v>4.3582360000000001E-2</v>
+      </c>
+      <c r="O15">
         <v>3687549.0855038119</v>
       </c>
-      <c r="N15">
+      <c r="P15">
         <v>8</v>
       </c>
-      <c r="O15">
+      <c r="Q15">
         <v>9025</v>
       </c>
-      <c r="P15" t="b">
+      <c r="R15" t="b">
         <v>1</v>
       </c>
-      <c r="Q15" t="s">
+      <c r="S15" t="s">
         <v>32</v>
       </c>
-      <c r="R15">
+      <c r="T15">
         <v>190258660</v>
       </c>
-      <c r="S15">
+      <c r="U15" s="4">
+        <f t="shared" si="2"/>
+        <v>0.19025866</v>
+      </c>
+      <c r="V15">
         <v>4442726.4335090453</v>
       </c>
-      <c r="U15">
-        <f t="shared" si="0"/>
+      <c r="X15">
+        <f t="shared" si="3"/>
         <v>0.70044052863436124</v>
       </c>
-      <c r="V15">
-        <f t="shared" si="1"/>
+      <c r="Y15">
+        <f t="shared" si="4"/>
         <v>0.79515418502202639</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>8</v>
       </c>
@@ -4352,55 +4570,67 @@
       <c r="F16">
         <v>6631693500</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="5">
+        <f t="shared" si="0"/>
+        <v>6.6316934999999999</v>
+      </c>
+      <c r="H16">
         <v>155159686.43238169</v>
       </c>
-      <c r="H16">
+      <c r="I16">
         <v>9</v>
       </c>
-      <c r="I16">
+      <c r="J16">
         <v>8075</v>
       </c>
-      <c r="J16" t="b">
+      <c r="K16" t="b">
         <v>1</v>
       </c>
-      <c r="K16" t="s">
+      <c r="L16" t="s">
         <v>34</v>
       </c>
-      <c r="L16">
+      <c r="M16">
         <v>45893360</v>
       </c>
-      <c r="M16">
+      <c r="N16" s="4">
+        <f t="shared" si="1"/>
+        <v>4.5893360000000001E-2</v>
+      </c>
+      <c r="O16">
         <v>5517285.5801562415</v>
       </c>
-      <c r="N16">
+      <c r="P16">
         <v>9</v>
       </c>
-      <c r="O16">
+      <c r="Q16">
         <v>9025</v>
       </c>
-      <c r="P16" t="b">
+      <c r="R16" t="b">
         <v>1</v>
       </c>
-      <c r="Q16" t="s">
+      <c r="S16" t="s">
         <v>35</v>
       </c>
-      <c r="R16">
+      <c r="T16">
         <v>206657280</v>
       </c>
-      <c r="S16">
+      <c r="U16" s="4">
+        <f t="shared" si="2"/>
+        <v>0.20665728</v>
+      </c>
+      <c r="V16">
         <v>2685045.119173978</v>
       </c>
-      <c r="U16">
-        <f t="shared" si="0"/>
+      <c r="X16">
+        <f t="shared" si="3"/>
         <v>0.70370370370370372</v>
       </c>
-      <c r="V16">
-        <f t="shared" si="1"/>
+      <c r="Y16">
+        <f t="shared" si="4"/>
         <v>0.78649237472766886</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>9</v>
       </c>
@@ -4419,55 +4649,67 @@
       <c r="F17">
         <v>6657019420</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="5">
+        <f t="shared" si="0"/>
+        <v>6.6570194200000001</v>
+      </c>
+      <c r="H17">
         <v>173239407.04079711</v>
       </c>
-      <c r="H17">
+      <c r="I17">
         <v>10</v>
       </c>
-      <c r="I17">
+      <c r="J17">
         <v>8475</v>
       </c>
-      <c r="J17" t="b">
+      <c r="K17" t="b">
         <v>1</v>
       </c>
-      <c r="K17" t="s">
+      <c r="L17" t="s">
         <v>37</v>
       </c>
-      <c r="L17">
+      <c r="M17">
         <v>28554100</v>
       </c>
-      <c r="M17">
+      <c r="N17" s="4">
+        <f t="shared" si="1"/>
+        <v>2.8554099999999999E-2</v>
+      </c>
+      <c r="O17">
         <v>1374291.004481948</v>
       </c>
-      <c r="N17">
+      <c r="P17">
         <v>10</v>
       </c>
-      <c r="O17">
+      <c r="Q17">
         <v>9025</v>
       </c>
-      <c r="P17" t="b">
+      <c r="R17" t="b">
         <v>1</v>
       </c>
-      <c r="Q17" t="s">
+      <c r="S17" t="s">
         <v>38</v>
       </c>
-      <c r="R17">
+      <c r="T17">
         <v>218618860</v>
       </c>
-      <c r="S17">
+      <c r="U17" s="4">
+        <f t="shared" si="2"/>
+        <v>0.21861886</v>
+      </c>
+      <c r="V17">
         <v>9207895.62022724</v>
       </c>
-      <c r="U17">
-        <f t="shared" si="0"/>
+      <c r="X17">
+        <f t="shared" si="3"/>
         <v>0.7306034482758621</v>
       </c>
-      <c r="V17">
-        <f t="shared" si="1"/>
+      <c r="Y17">
+        <f t="shared" si="4"/>
         <v>0.77801724137931039</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>10</v>
       </c>
@@ -4486,55 +4728,67 @@
       <c r="F18">
         <v>9702281300</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="5">
+        <f t="shared" si="0"/>
+        <v>9.7022812999999992</v>
+      </c>
+      <c r="H18">
         <v>316659027.06926727</v>
       </c>
-      <c r="H18">
+      <c r="I18">
         <v>11</v>
       </c>
-      <c r="I18">
+      <c r="J18">
         <v>7925</v>
       </c>
-      <c r="J18" t="b">
+      <c r="K18" t="b">
         <v>1</v>
       </c>
-      <c r="K18" t="s">
+      <c r="L18" t="s">
         <v>40</v>
       </c>
-      <c r="L18">
+      <c r="M18">
         <v>29544700</v>
       </c>
-      <c r="M18">
+      <c r="N18" s="4">
+        <f t="shared" si="1"/>
+        <v>2.95447E-2</v>
+      </c>
+      <c r="O18">
         <v>2511521.0381360529</v>
       </c>
-      <c r="N18">
+      <c r="P18">
         <v>11</v>
       </c>
-      <c r="O18">
+      <c r="Q18">
         <v>8975</v>
       </c>
-      <c r="P18" t="b">
+      <c r="R18" t="b">
         <v>1</v>
       </c>
-      <c r="Q18" t="s">
+      <c r="S18" t="s">
         <v>41</v>
       </c>
-      <c r="R18">
+      <c r="T18">
         <v>220807920</v>
       </c>
-      <c r="S18">
+      <c r="U18" s="4">
+        <f t="shared" si="2"/>
+        <v>0.22080791999999999</v>
+      </c>
+      <c r="V18">
         <v>6106007.3765104478</v>
       </c>
-      <c r="U18">
-        <f t="shared" si="0"/>
+      <c r="X18">
+        <f t="shared" si="3"/>
         <v>0.68318965517241381</v>
       </c>
-      <c r="V18">
-        <f t="shared" si="1"/>
+      <c r="Y18">
+        <f t="shared" si="4"/>
         <v>0.77370689655172409</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>11</v>
       </c>
@@ -4553,59 +4807,79 @@
       <c r="F19">
         <v>9517605000</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="5">
+        <f t="shared" si="0"/>
+        <v>9.5176049999999996</v>
+      </c>
+      <c r="H19">
         <v>71575243.936887845</v>
       </c>
-      <c r="H19">
+      <c r="I19">
         <v>12</v>
       </c>
-      <c r="I19">
+      <c r="J19">
         <v>7425</v>
       </c>
-      <c r="J19" t="b">
+      <c r="K19" t="b">
         <v>1</v>
       </c>
-      <c r="K19" t="s">
+      <c r="L19" t="s">
         <v>43</v>
       </c>
-      <c r="L19">
+      <c r="M19">
         <v>141190560</v>
       </c>
-      <c r="M19">
+      <c r="N19" s="4">
+        <f t="shared" si="1"/>
+        <v>0.14119055999999999</v>
+      </c>
+      <c r="O19">
         <v>4807991.0865142001</v>
       </c>
-      <c r="N19">
+      <c r="P19">
         <v>12</v>
       </c>
-      <c r="O19">
+      <c r="Q19">
         <v>8400</v>
       </c>
-      <c r="P19" t="b">
+      <c r="R19" t="b">
         <v>1</v>
       </c>
-      <c r="Q19" t="s">
+      <c r="S19" t="s">
         <v>44</v>
       </c>
-      <c r="R19">
+      <c r="T19">
         <v>225462480</v>
       </c>
-      <c r="S19">
+      <c r="U19" s="4">
+        <f t="shared" si="2"/>
+        <v>0.22546247999999999</v>
+      </c>
+      <c r="V19">
         <v>5057501.4772118451</v>
       </c>
-      <c r="U19">
-        <f t="shared" si="0"/>
+      <c r="X19">
+        <f t="shared" si="3"/>
         <v>0.64008620689655171</v>
       </c>
-      <c r="V19">
-        <f t="shared" si="1"/>
+      <c r="Y19">
+        <f t="shared" si="4"/>
         <v>0.72413793103448276</v>
+      </c>
+    </row>
+    <row r="56" spans="11:22" x14ac:dyDescent="0.25">
+      <c r="K56" t="s">
+        <v>50</v>
+      </c>
+      <c r="V56" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="N5:S5"/>
-    <mergeCell ref="H5:M5"/>
-    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="P5:V5"/>
+    <mergeCell ref="I5:O5"/>
+    <mergeCell ref="B5:H5"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>

</xml_diff>